<commit_message>
Finish updating all scim provisioning test images with inverted spotlight
</commit_message>
<xml_diff>
--- a/packages/@okta/vuepress-site/.vuepress/public/standards/SCIM/SCIMFiles/okta-scim-test-plan.xlsx
+++ b/packages/@okta/vuepress-site/.vuepress/public/standards/SCIM/SCIMFiles/okta-scim-test-plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardopedayo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alatiniuk/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC1F0AF-265D-0B43-99A6-788EB6019988}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{05296C65-1161-4D49-8B06-E848CB518D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1069,22 +1069,6 @@
     <t>Verify Push Groups &gt; Push Now</t>
   </si>
   <si>
-    <t>1. Sign in to Okta as **Admin**
-2. Go to https:&lt;domain&gt;/admin/dashboard
-3. From the **Dashboard** page, search your application
-4. From the **Application** page, select the **Push Groups** tab
-5. Under **Push Groups** tab, click **Push Groups**
-6. Click **Find groups by name**
-7. Enter a group to push
-8. Under **Match result &amp; push action**, select  **Create Group**
-9. Click **Save**
-10. From the **Push Groups** tab, click **Active**
-11. Sign in to **Downstream Application** and observe the created group
-12. From the **Downstream application** add several new members to the group, members should not be provisioned from Okta
-13. From the **Push Groups** tab in Okta, click **Active**
-114. Click *Push Now**</t>
-  </si>
-  <si>
     <t>Push Now serves to "force" a push in the rare occurrence when the state of Okta and the target app are no longer in sync. This action performs a full overwrite of the overall membership and makes Okta the master for the group. The exception to this is Active Directory, which only pushes the newest members to the group, and does not overwrite overall membership.</t>
   </si>
   <si>
@@ -1637,6 +1621,21 @@
   </si>
   <si>
     <t xml:space="preserve">Deactivating end user revokes their app assignments, the end user is listed as Deactivated under the Status column in User Profile. </t>
+  </si>
+  <si>
+    <t>1. Log in to Okta as Admin
+2. Go to https:/admin/dashboard
+3. From the Dashboard page, search your application
+4. From the Application page, select the Push Groups tab
+5. Under Push Groups tab, click Push Groups
+6. Click Find groups by name
+7. Enter a group to push
+8. Under Match result &amp; push action, select  Create Group
+9. Click Save
+10. Log in to Downstream Application and observe the created group
+11. From the Downstream application add several new members to the group, members should not be provisioned from OKTA
+12. From the Push Groups tab in OKTA, click Active
+13. Click *Push Now**</t>
   </si>
 </sst>
 </file>
@@ -1941,8 +1940,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2796,7 +2795,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="272" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="238" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>201</v>
       </c>
@@ -2810,58 +2809,58 @@
         <v>193</v>
       </c>
       <c r="E42" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="187" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>194</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="372" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>192</v>
@@ -2870,18 +2869,18 @@
         <v>193</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>192</v>
@@ -2890,58 +2889,58 @@
         <v>193</v>
       </c>
       <c r="E46" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>192</v>
@@ -2950,178 +2949,178 @@
         <v>193</v>
       </c>
       <c r="E49" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="340" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E51" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="340" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E52" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E53" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D55" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="F55" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="238" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="F56" s="3" t="s">
         <v>263</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="323" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E57" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="372" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>192</v>
@@ -3130,18 +3129,18 @@
         <v>193</v>
       </c>
       <c r="E58" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="323" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>192</v>
@@ -3150,70 +3149,70 @@
         <v>193</v>
       </c>
       <c r="E59" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E60" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="204" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="F61" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="238" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="E62" s="4" t="s">
+      <c r="F62" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>